<commit_message>
Updated JPN model - 2025-08-28 02:08
</commit_message>
<xml_diff>
--- a/VerveStacks_JPN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_JPN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_JPN\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CC6D074-C618-4A53-96FC-F642127BB42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DBE528E-2E8A-4752-BA37-86C48E5BB622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -847,18 +847,18 @@
     <t>wind resource -- CF class won-JPN_43 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-JPN_43_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-JPN_43 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-JPN_43_c5</t>
   </si>
   <si>
     <t>wind resource -- CF class won-JPN_43 -- cost class 5</t>
   </si>
   <si>
-    <t>e_won-JPN_43_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-JPN_43 -- cost class 4</t>
-  </si>
-  <si>
     <t>e_won-JPN_43_c3</t>
   </si>
   <si>
@@ -1117,18 +1117,18 @@
     <t>wind resource -- CF class won-JPN_31 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-JPN_31_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-JPN_31 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-JPN_31_c5</t>
   </si>
   <si>
     <t>wind resource -- CF class won-JPN_31 -- cost class 5</t>
   </si>
   <si>
-    <t>e_won-JPN_31_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-JPN_31 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_won-JPN_31_c4</t>
   </si>
   <si>
@@ -1243,22 +1243,22 @@
     <t>wind resource -- CF class won-JPN_27 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-JPN_27_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-JPN_27 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_won-JPN_27_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-JPN_27 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-JPN_27_c5</t>
   </si>
   <si>
     <t>wind resource -- CF class won-JPN_27 -- cost class 5</t>
-  </si>
-  <si>
-    <t>e_won-JPN_27_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-JPN_27 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-JPN_27_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-JPN_27 -- cost class 4</t>
   </si>
   <si>
     <t>e_won-JPN_26_c1</t>
@@ -2785,7 +2785,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DE7228C-72BC-7C62-B249-AE737F67D6ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02C3CDD-3E27-7399-F4B8-B481D8460168}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2840,7 +2840,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{399291D4-89CC-58D6-0164-2DC0869A99B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BC400C-97EC-B9D6-3319-3E48FA7E4211}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2895,7 +2895,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20ABEF1F-EDA1-9443-BB85-B3AF52EF52C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AB1E62B-F122-97DC-4B6A-ED859A6D136F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2950,7 +2950,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F0F1161-2C05-35AA-C34A-6757D259C8F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DBB840E-8462-A337-6674-335439D96908}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6880,7 +6880,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA46359-AB37-4D71-96B5-28AB4CDEAF1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D5E5E6-D090-48A9-9A33-8FC2179969A3}">
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8080,7 +8080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E746E7-D58E-4E6F-9CF9-E78ADAE98B34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AE3CDB-23A4-4A77-B43C-B1420D5D59AA}">
   <dimension ref="A1:P142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8274,16 +8274,16 @@
         <v>513</v>
       </c>
       <c r="M6" s="160">
-        <v>6.7499999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="N6" s="158">
         <v>0.42699999999999999</v>
       </c>
       <c r="O6" s="161">
-        <v>100.81671438172461</v>
+        <v>100.72597028009119</v>
       </c>
       <c r="P6" s="160">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -8315,16 +8315,16 @@
         <v>513</v>
       </c>
       <c r="M7" s="162">
-        <v>3.0000000000000001E-3</v>
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="N7" s="159">
         <v>0.42699999999999999</v>
       </c>
       <c r="O7" s="163">
-        <v>100.72597028009119</v>
+        <v>100.81671438172461</v>
       </c>
       <c r="P7" s="162">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -10119,16 +10119,16 @@
         <v>513</v>
       </c>
       <c r="M51" s="162">
-        <v>7.5000000000000002E-4</v>
+        <v>6.3E-2</v>
       </c>
       <c r="N51" s="159">
         <v>0.313</v>
       </c>
       <c r="O51" s="163">
-        <v>87.256420853104913</v>
+        <v>59.397981651653055</v>
       </c>
       <c r="P51" s="162">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="2:16">
@@ -10160,16 +10160,16 @@
         <v>513</v>
       </c>
       <c r="M52" s="160">
-        <v>6.3E-2</v>
+        <v>7.5000000000000002E-4</v>
       </c>
       <c r="N52" s="158">
         <v>0.313</v>
       </c>
       <c r="O52" s="161">
-        <v>59.397981651653055</v>
+        <v>87.256420853104913</v>
       </c>
       <c r="P52" s="160">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="2:16">
@@ -10980,16 +10980,16 @@
         <v>513</v>
       </c>
       <c r="M72" s="160">
-        <v>1.51725</v>
+        <v>4.8937499999999998</v>
       </c>
       <c r="N72" s="158">
         <v>0.26600000000000001</v>
       </c>
       <c r="O72" s="161">
-        <v>175.6471767639768</v>
+        <v>72.834109613341482</v>
       </c>
       <c r="P72" s="160">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="2:16">
@@ -11021,16 +11021,16 @@
         <v>513</v>
       </c>
       <c r="M73" s="162">
-        <v>4.8937499999999998</v>
+        <v>0.70574999999999999</v>
       </c>
       <c r="N73" s="159">
         <v>0.26600000000000001</v>
       </c>
       <c r="O73" s="163">
-        <v>72.834109613341482</v>
+        <v>92.253347362887894</v>
       </c>
       <c r="P73" s="162">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="2:16">
@@ -11062,16 +11062,16 @@
         <v>513</v>
       </c>
       <c r="M74" s="160">
-        <v>0.70574999999999999</v>
+        <v>1.51725</v>
       </c>
       <c r="N74" s="158">
         <v>0.26600000000000001</v>
       </c>
       <c r="O74" s="161">
-        <v>92.253347362887894</v>
+        <v>175.6471767639768</v>
       </c>
       <c r="P74" s="160">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="2:16">
@@ -13872,7 +13872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0806A7E2-F711-4675-AA30-05C97DEE9E25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082E87E6-9648-46E8-B7A3-27072B946E57}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated JPN model - 2025-09-06 00:30
</commit_message>
<xml_diff>
--- a/VerveStacks_JPN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_JPN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_JPN\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{779114C4-A5C5-41B4-950B-0885A4D03F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93E32453-6AF3-4421-8F1C-B60B5F625A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8535,7 +8535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9EADEB-C620-459A-94BA-7563650F7522}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF2029D-B851-4EA7-B1DC-A3E4CD2B9C63}">
   <dimension ref="B9:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9696,7 +9696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23AC0A5F-4D0B-4B92-A141-446DBB5A9CB9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD0573D-357A-41FB-AD79-593F1362E8D7}">
   <dimension ref="B9:AB241"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26459,7 +26459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C1E1FF-E121-4A74-861E-67114941348C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF02795-4EAC-4852-9FB4-92C827F616FD}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>